<commit_message>
Revert "Merge branch 'main' into 2025-01/linfergar"
This reverts commit 2f3822c8a57451d6730aa222c2702cc715463f1f, reversing
changes made to ca43f93df1466107c3114c4666f7aeba3ebf1faa.
</commit_message>
<xml_diff>
--- a/Exams/Exam-02/Program_CheckList.xlsx
+++ b/Exams/Exam-02/Program_CheckList.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Personal\Cursos\ServicesDevelopment\Repository\Exams\Exam-02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Repositories\ServicesDevelopment\Exams\Exam-02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10381F2C-2EBC-4C0C-B8B3-2E8F461107FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052E2512-6811-4656-B3BA-FF12AC56DC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4164" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -45,6 +56,9 @@
     <t>Compila sin Errores</t>
   </si>
   <si>
+    <t>Cumple con Clean Architecture (Plural,Metodos CRUD, Manejoa los errores)</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
@@ -55,9 +69,6 @@
   </si>
   <si>
     <t>Tests</t>
-  </si>
-  <si>
-    <t>Cumple con Clean Architecture (Plural,Metodos CRUD, Manejo de los errores)</t>
   </si>
 </sst>
 </file>
@@ -477,7 +488,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -521,7 +532,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="16">
         <f>SUM(C4:C5)</f>
@@ -538,7 +549,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="15">
@@ -549,7 +560,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="15">
@@ -560,7 +571,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="9">

</xml_diff>

<commit_message>
Revert "Merge branch 'main' into 2025-01/andlasper"
This reverts commit b1aa7e6df1d9df170c1cd750f6c5075c2a7cf8b9, reversing
changes made to 9a5904f51b2ef29cff051ace97d215eecb6cf8d3.
</commit_message>
<xml_diff>
--- a/Exams/Exam-02/Program_CheckList.xlsx
+++ b/Exams/Exam-02/Program_CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Personal\Cursos\ServicesDevelopment\Repository\Exams\Exam-02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10381F2C-2EBC-4C0C-B8B3-2E8F461107FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7531243D-F371-4E11-AB98-AD2291A4D84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-4164" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Creterio</t>
   </si>
@@ -45,6 +45,9 @@
     <t>Compila sin Errores</t>
   </si>
   <si>
+    <t>Cumple con Clean Architecture (Plural,Metodos CRUD, Manejoa los errores)</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
@@ -57,7 +60,7 @@
     <t>Tests</t>
   </si>
   <si>
-    <t>Cumple con Clean Architecture (Plural,Metodos CRUD, Manejo de los errores)</t>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -521,7 +524,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="16">
         <f>SUM(C4:C5)</f>
@@ -538,7 +541,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="15">
@@ -549,7 +552,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="15">
@@ -560,7 +563,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="9">
@@ -581,7 +584,9 @@
         <f>SUM(D2:D6)</f>
         <v>5</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>

</xml_diff>